<commit_message>
Lots of fixes to joints and models
</commit_message>
<xml_diff>
--- a/human_measurements.xlsx
+++ b/human_measurements.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="121">
   <si>
     <t>Pounds to Kilograms</t>
   </si>
@@ -288,9 +288,6 @@
   </si>
   <si>
     <t>Offset Z</t>
-  </si>
-  <si>
-    <t>TODO: Re-derive X Y Z</t>
   </si>
   <si>
     <t>Note: Offset values include movement of the entire model</t>
@@ -494,8 +491,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="559">
+  <cellStyleXfs count="607">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1091,7 +1136,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="559">
+  <cellStyles count="607">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1371,6 +1416,30 @@
     <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="578" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="580" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="596" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="604" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="606" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1650,6 +1719,30 @@
     <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="575" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="577" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="579" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="581" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="585" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="595" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="603" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="605" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -3543,11 +3636,12 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="10" max="10" width="48.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3573,11 +3667,8 @@
       <c r="G1" t="s">
         <v>87</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>88</v>
-      </c>
-      <c r="J1" t="s">
-        <v>89</v>
       </c>
       <c r="K1" t="s">
         <v>85</v>
@@ -3589,12 +3680,12 @@
         <v>87</v>
       </c>
       <c r="N1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="18">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2">
         <f>Height!$E$5/2</f>
@@ -3631,14 +3722,13 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <f>-1 * Width!$C$3 / 2</f>
-        <v>-8.5500000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -3649,7 +3739,7 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F20" si="1">C3+$L$2</f>
-        <v>-0.27330399999999999</v>
+        <v>-0.187804</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G20" si="2">D3+$M$2</f>
@@ -3658,7 +3748,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4">
         <f>Height!$E$5/2</f>
@@ -3686,14 +3776,13 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <f>1 * Width!$C$3 / 2</f>
-        <v>8.5500000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3704,7 +3793,7 @@
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>-0.10230399999999999</v>
+        <v>-0.187804</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
@@ -3713,7 +3802,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3741,18 +3830,17 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <f>-1 * Width!$C$3 / 2</f>
-        <v>-8.5500000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <f>Height!$E$6</f>
-        <v>0.40899999999999997</v>
+        <f>Height!$E$6/2</f>
+        <v>0.20449999999999999</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
@@ -3760,16 +3848,16 @@
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>-0.27330399999999999</v>
+        <v>-0.187804</v>
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>0.40899999999999997</v>
+        <v>0.20449999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3797,18 +3885,17 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <f>1 * Width!$C$3 / 2</f>
-        <v>8.5500000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <f>Height!$E$6</f>
-        <v>0.40899999999999997</v>
+        <f>Height!$E$6/2</f>
+        <v>0.20449999999999999</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
@@ -3816,16 +3903,16 @@
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>-0.10230399999999999</v>
+        <v>-0.187804</v>
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>0.40899999999999997</v>
+        <v>0.20449999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3853,18 +3940,17 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11">
-        <f>-1 * Width!$C$3 / 2</f>
-        <v>-8.5500000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <f>Height!$E$6+Height!$E$7</f>
-        <v>0.84299999999999997</v>
+        <f>Height!$E$7/2</f>
+        <v>0.217</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
@@ -3872,16 +3958,16 @@
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>-0.27330399999999999</v>
+        <v>-0.187804</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>0.84299999999999997</v>
+        <v>0.217</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -3909,18 +3995,17 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <f>1 * Width!$C$3 / 2</f>
-        <v>8.5500000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <f>Height!$E$6+Height!$E$7</f>
-        <v>0.84299999999999997</v>
+        <f>Height!$E$7/2</f>
+        <v>0.217</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
@@ -3928,16 +4013,16 @@
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>-0.10230399999999999</v>
+        <v>-0.187804</v>
       </c>
       <c r="G13">
         <f t="shared" si="2"/>
-        <v>0.84299999999999997</v>
+        <v>0.217</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -3964,7 +4049,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -3973,8 +4058,7 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <f>Height!$E$6+Height!$E$7</f>
-        <v>0.84299999999999997</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
@@ -3986,12 +4070,12 @@
       </c>
       <c r="G15">
         <f t="shared" si="2"/>
-        <v>0.84299999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4018,7 +4102,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4027,8 +4111,7 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <f>Height!$E$6+Height!$E$7+Height!$E$9</f>
-        <v>1.2189999999999999</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
@@ -4040,12 +4123,12 @@
       </c>
       <c r="G17">
         <f t="shared" si="2"/>
-        <v>1.2189999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4072,7 +4155,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -4081,8 +4164,8 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <f>Height!$E$6+Height!$E$7+Height!$E$9</f>
-        <v>1.2189999999999999</v>
+        <f>-Height!$E$8/2</f>
+        <v>-0.16250000000000001</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
@@ -4094,12 +4177,12 @@
       </c>
       <c r="G19">
         <f t="shared" si="2"/>
-        <v>1.2189999999999999</v>
+        <v>-0.16250000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -4125,7 +4208,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -4153,18 +4236,17 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22">
-        <f>-1 * Width!$C$2 / 2</f>
-        <v>-8.1500000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <f>Height!$E$6+Height!$E$7+Height!$E$9</f>
-        <v>1.2189999999999999</v>
+        <f>-Height!$E$4/2</f>
+        <v>-0.151</v>
       </c>
       <c r="E22">
         <f t="shared" si="3"/>
@@ -4172,16 +4254,16 @@
       </c>
       <c r="F22">
         <f t="shared" si="4"/>
-        <v>-0.26930399999999999</v>
+        <v>-0.187804</v>
       </c>
       <c r="G22">
         <f t="shared" si="5"/>
-        <v>1.2189999999999999</v>
+        <v>-0.151</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -4209,18 +4291,17 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24">
-        <f>1 * Width!$C$2 / 2</f>
-        <v>8.1500000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <f>Height!$E$6+Height!$E$7+Height!$E$9</f>
-        <v>1.2189999999999999</v>
+        <f>-Height!$E$4/2</f>
+        <v>-0.151</v>
       </c>
       <c r="E24">
         <f t="shared" si="3"/>
@@ -4228,16 +4309,16 @@
       </c>
       <c r="F24">
         <f t="shared" si="4"/>
-        <v>-0.106304</v>
+        <v>-0.187804</v>
       </c>
       <c r="G24">
         <f t="shared" si="5"/>
-        <v>1.2189999999999999</v>
+        <v>-0.151</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -4265,18 +4346,17 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26">
-        <f>-1 * Width!$C$2 / 2</f>
-        <v>-8.1500000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <f>Height!$E$6+Height!$E$7+Height!$E$9+Height!$E$4</f>
-        <v>1.5209999999999999</v>
+        <f>-Height!$E$3/2</f>
+        <v>-0.13600000000000001</v>
       </c>
       <c r="E26">
         <f t="shared" si="3"/>
@@ -4284,16 +4364,16 @@
       </c>
       <c r="F26">
         <f t="shared" si="4"/>
-        <v>-0.26930399999999999</v>
+        <v>-0.187804</v>
       </c>
       <c r="G26">
         <f t="shared" si="5"/>
-        <v>1.5209999999999999</v>
+        <v>-0.13600000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -4321,18 +4401,17 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="C28">
-        <f>1 * Width!$C$2 / 2</f>
-        <v>8.1500000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <f>Height!$E$6+Height!$E$7+Height!$E$9+Height!$E$4</f>
-        <v>1.5209999999999999</v>
+        <f>-Height!$E$3/2</f>
+        <v>-0.13600000000000001</v>
       </c>
       <c r="E28">
         <f t="shared" si="3"/>
@@ -4340,16 +4419,16 @@
       </c>
       <c r="F28">
         <f t="shared" si="4"/>
-        <v>-0.106304</v>
+        <v>-0.187804</v>
       </c>
       <c r="G28">
         <f t="shared" si="5"/>
-        <v>1.5209999999999999</v>
+        <v>-0.13600000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -4377,18 +4456,17 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30">
-        <f>-1 * Width!$C$2 / 2</f>
-        <v>-8.1500000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <f>Height!$E$6+Height!$E$7+Height!$E$9+Height!$E$4+Height!$E$3</f>
-        <v>1.7929999999999999</v>
+        <f>-Height!$E$2/2</f>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="E30">
         <f t="shared" si="3"/>
@@ -4396,16 +4474,16 @@
       </c>
       <c r="F30">
         <f t="shared" si="4"/>
-        <v>-0.26930399999999999</v>
+        <v>-0.187804</v>
       </c>
       <c r="G30">
         <f t="shared" si="5"/>
-        <v>1.7929999999999999</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -4433,18 +4511,17 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="C32">
-        <f>1 * Width!$C$2 / 2</f>
-        <v>8.1500000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <f>Height!$E$6+Height!$E$7+Height!$E$9+Height!$E$4+Height!$E$3</f>
-        <v>1.7929999999999999</v>
+        <f>-Height!$E$2/2</f>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="E32">
         <f t="shared" si="6"/>
@@ -4452,11 +4529,11 @@
       </c>
       <c r="F32">
         <f t="shared" ref="F32" si="9">C32+$L$2</f>
-        <v>-0.106304</v>
+        <v>-0.187804</v>
       </c>
       <c r="G32">
         <f t="shared" ref="G32" si="10">D32+$M$2</f>
-        <v>1.7929999999999999</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Check and fix all limit values
</commit_message>
<xml_diff>
--- a/human_measurements.xlsx
+++ b/human_measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="10820" yWindow="1380" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Weight" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Width" sheetId="4" r:id="rId4"/>
     <sheet name="Circumference" sheetId="5" r:id="rId5"/>
     <sheet name="Poses" sheetId="6" r:id="rId6"/>
+    <sheet name="Joint Limits" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="164">
   <si>
     <t>Pounds to Kilograms</t>
   </si>
@@ -371,9 +372,6 @@
     <t>right_forearm</t>
   </si>
   <si>
-    <t>TODO: Fix base human model</t>
-  </si>
-  <si>
     <t>right_elbow</t>
   </si>
   <si>
@@ -387,13 +385,145 @@
   </si>
   <si>
     <t>right_wrist</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Upper</t>
+  </si>
+  <si>
+    <t>Table 5</t>
+  </si>
+  <si>
+    <t>Pitch (Degrees)</t>
+  </si>
+  <si>
+    <t>Yaw (Degrees)</t>
+  </si>
+  <si>
+    <t>Pitch (Rad)</t>
+  </si>
+  <si>
+    <t>Yaw (Rad)</t>
+  </si>
+  <si>
+    <t>Table 6</t>
+  </si>
+  <si>
+    <t>Table 8</t>
+  </si>
+  <si>
+    <t>Table 9</t>
+  </si>
+  <si>
+    <t>Table 10</t>
+  </si>
+  <si>
+    <t>Table 11</t>
+  </si>
+  <si>
+    <t>Table 12</t>
+  </si>
+  <si>
+    <t>Table 13</t>
+  </si>
+  <si>
+    <t>Table 14</t>
+  </si>
+  <si>
+    <t>Table 15</t>
+  </si>
+  <si>
+    <t>Table 16</t>
+  </si>
+  <si>
+    <t>Table 17</t>
+  </si>
+  <si>
+    <t>Table 18</t>
+  </si>
+  <si>
+    <t>Table 19</t>
+  </si>
+  <si>
+    <t>Table 20</t>
+  </si>
+  <si>
+    <t>Table 21</t>
+  </si>
+  <si>
+    <t>Table 22</t>
+  </si>
+  <si>
+    <t>Table 23</t>
+  </si>
+  <si>
+    <t>Table 24</t>
+  </si>
+  <si>
+    <t>Table 25</t>
+  </si>
+  <si>
+    <t>Table 26</t>
+  </si>
+  <si>
+    <t>Table 27</t>
+  </si>
+  <si>
+    <t>Table 28</t>
+  </si>
+  <si>
+    <t>Table 29</t>
+  </si>
+  <si>
+    <t>Table 30</t>
+  </si>
+  <si>
+    <t>Table 31</t>
+  </si>
+  <si>
+    <t>Table 32</t>
+  </si>
+  <si>
+    <t>Table 33</t>
+  </si>
+  <si>
+    <t>Table 34</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Currently locking neck movement</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Selected Standing/voluntary measurement</t>
+  </si>
+  <si>
+    <t>No yaw given for ankle</t>
+  </si>
+  <si>
+    <t>Base measurements. Ignoring rotation</t>
+  </si>
+  <si>
+    <t>Ignoring rotation</t>
+  </si>
+  <si>
+    <t>Table 5 - Median</t>
+  </si>
+  <si>
+    <t>Roll (Rad)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -436,6 +566,16 @@
       <sz val="15"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="TimesNewRoman"/>
     </font>
   </fonts>
   <fills count="4">
@@ -491,7 +631,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="607">
+  <cellStyleXfs count="669">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1099,8 +1239,70 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1135,8 +1337,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="607">
+  <cellStyles count="669">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1440,6 +1647,37 @@
     <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="604" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="608" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="610" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="612" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="614" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="620" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="624" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="626" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="628" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="630" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="632" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="634" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="636" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="638" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="664" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="668" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1743,6 +1981,37 @@
     <cellStyle name="Hyperlink" xfId="601" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="603" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="605" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="607" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="609" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="611" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="613" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="615" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="617" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="619" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="621" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="623" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="625" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="627" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="629" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="631" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="633" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="635" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="637" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="639" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="641" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="649" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="651" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="653" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="655" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="663" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="665" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="667" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -2811,14 +3080,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="50" customWidth="1"/>
     <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -3301,6 +3572,14 @@
         <f>D3*2+D4*2+D5*2+D6*2+D7*2+D8*2+D9+D10</f>
         <v>74.599999999999994</v>
       </c>
+    </row>
+    <row r="16" spans="1:15" ht="16">
+      <c r="C16" s="18"/>
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="2:3" ht="16">
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3633,10 +3912,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3645,7 +3924,7 @@
     <col min="10" max="10" width="48.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -3679,11 +3958,8 @@
       <c r="M1" t="s">
         <v>87</v>
       </c>
-      <c r="N1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="18">
+    </row>
+    <row r="2" spans="1:13" ht="18">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -3720,7 +3996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -3746,7 +4022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -3774,7 +4050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -3800,7 +4076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -3828,7 +4104,7 @@
         <v>0.20449999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>94</v>
       </c>
@@ -3855,7 +4131,7 @@
         <v>0.20449999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>95</v>
       </c>
@@ -3883,7 +4159,7 @@
         <v>0.20449999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -3910,7 +4186,7 @@
         <v>0.20449999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>97</v>
       </c>
@@ -3938,7 +4214,7 @@
         <v>0.626</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>98</v>
       </c>
@@ -3965,7 +4241,7 @@
         <v>0.217</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>99</v>
       </c>
@@ -3993,7 +4269,7 @@
         <v>0.626</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>100</v>
       </c>
@@ -4020,7 +4296,7 @@
         <v>0.217</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>101</v>
       </c>
@@ -4047,7 +4323,7 @@
         <v>0.84299999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>102</v>
       </c>
@@ -4073,7 +4349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>103</v>
       </c>
@@ -4401,7 +4677,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -4428,7 +4704,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -4456,7 +4732,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -4483,7 +4759,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -4511,7 +4787,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -4534,6 +4810,767 @@
       <c r="G32">
         <f t="shared" ref="G32" si="10">D32+$M$2</f>
         <v>-3.5000000000000003E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2">
+        <v>-39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2">
+        <f>RADIANS(C2)</f>
+        <v>-0.68067840827778847</v>
+      </c>
+      <c r="F2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3">
+        <v>41.6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E31" si="0">RADIANS(C3)</f>
+        <v>0.7260569688296411</v>
+      </c>
+      <c r="F3" t="s">
+        <v>157</v>
+      </c>
+      <c r="H3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4">
+        <v>-39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>-0.68067840827778847</v>
+      </c>
+      <c r="F4" t="s">
+        <v>157</v>
+      </c>
+      <c r="H4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="B5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5">
+        <v>41.6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.7260569688296411</v>
+      </c>
+      <c r="F5" t="s">
+        <v>157</v>
+      </c>
+      <c r="H5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6">
+        <v>-123.8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>-2.1607176139689801</v>
+      </c>
+      <c r="F6" t="s">
+        <v>157</v>
+      </c>
+      <c r="H6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="B7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8">
+        <v>-123.8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>-2.1607176139689801</v>
+      </c>
+      <c r="F8" t="s">
+        <v>157</v>
+      </c>
+      <c r="H8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="B9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>157</v>
+      </c>
+      <c r="H9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>-27.7</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f>RADIANS(D10)</f>
+        <v>-0.48345620280242929</v>
+      </c>
+      <c r="H10" t="s">
+        <v>133</v>
+      </c>
+      <c r="I10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="B11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11">
+        <v>117.1</v>
+      </c>
+      <c r="D11">
+        <v>58</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>2.0437805540853597</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11:F19" si="1">RADIANS(D11)</f>
+        <v>1.0122909661567112</v>
+      </c>
+      <c r="H11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>-27.7</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>-0.48345620280242929</v>
+      </c>
+      <c r="H12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="B13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13">
+        <v>117.1</v>
+      </c>
+      <c r="D13">
+        <v>58</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>2.0437805540853597</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>1.0122909661567112</v>
+      </c>
+      <c r="H13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="B15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="B17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>141</v>
+      </c>
+      <c r="I18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="B19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20">
+        <v>-63</v>
+      </c>
+      <c r="D20">
+        <v>-50.8</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>-1.0995574287564276</v>
+      </c>
+      <c r="F20">
+        <f>RADIANS(D21)</f>
+        <v>2.3055799418845093</v>
+      </c>
+      <c r="H20" t="s">
+        <v>143</v>
+      </c>
+      <c r="I20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="B21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21">
+        <v>193.2</v>
+      </c>
+      <c r="D21">
+        <v>132.1</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>3.3719761148530445</v>
+      </c>
+      <c r="F21">
+        <f>RADIANS(D20)</f>
+        <v>-0.88662726001311931</v>
+      </c>
+      <c r="H21" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22">
+        <v>-63</v>
+      </c>
+      <c r="D22">
+        <v>-50.8</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>-1.0995574287564276</v>
+      </c>
+      <c r="F22">
+        <f>RADIANS(D22)</f>
+        <v>-0.88662726001311931</v>
+      </c>
+      <c r="H22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="B23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23">
+        <v>193.2</v>
+      </c>
+      <c r="D23">
+        <v>132.1</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>3.3719761148530445</v>
+      </c>
+      <c r="F23">
+        <f>RADIANS(D23)</f>
+        <v>2.3055799418845093</v>
+      </c>
+      <c r="H23" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>157</v>
+      </c>
+      <c r="H24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="B25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25">
+        <v>141</v>
+      </c>
+      <c r="D25" t="s">
+        <v>157</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>2.4609142453120048</v>
+      </c>
+      <c r="F25" t="s">
+        <v>157</v>
+      </c>
+      <c r="H25" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>157</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>157</v>
+      </c>
+      <c r="H26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="B27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27">
+        <v>141</v>
+      </c>
+      <c r="D27" t="s">
+        <v>157</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>2.4609142453120048</v>
+      </c>
+      <c r="F27" t="s">
+        <v>157</v>
+      </c>
+      <c r="H27" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28">
+        <v>-94.6</v>
+      </c>
+      <c r="D28">
+        <v>-25.1</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>-1.6510814723866356</v>
+      </c>
+      <c r="F28">
+        <f>RADIANS(D28)</f>
+        <v>-0.43807764225057672</v>
+      </c>
+      <c r="H28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="B29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29">
+        <v>102</v>
+      </c>
+      <c r="D29">
+        <v>46.3</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>1.7802358370342162</v>
+      </c>
+      <c r="F29">
+        <f>RADIANS(D29)</f>
+        <v>0.80808744367337448</v>
+      </c>
+      <c r="H29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30">
+        <v>-94.6</v>
+      </c>
+      <c r="D30">
+        <v>-25.1</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>-1.6510814723866356</v>
+      </c>
+      <c r="F30">
+        <f>RADIANS(D30)</f>
+        <v>-0.43807764225057672</v>
+      </c>
+      <c r="H30" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="B31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31">
+        <v>102</v>
+      </c>
+      <c r="D31">
+        <v>46.3</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>1.7802358370342162</v>
+      </c>
+      <c r="F31">
+        <f>RADIANS(D31)</f>
+        <v>0.80808744367337448</v>
+      </c>
+      <c r="H31" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add damping. Fix shoulder joints
</commit_message>
<xml_diff>
--- a/human_measurements.xlsx
+++ b/human_measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10820" yWindow="1380" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="2700" yWindow="2600" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Weight" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="165">
   <si>
     <t>Pounds to Kilograms</t>
   </si>
@@ -510,13 +510,16 @@
     <t>Base measurements. Ignoring rotation</t>
   </si>
   <si>
-    <t>Ignoring rotation</t>
-  </si>
-  <si>
     <t>Table 5 - Median</t>
   </si>
   <si>
     <t>Roll (Rad)</t>
+  </si>
+  <si>
+    <t>Hip cannot go below 0</t>
+  </si>
+  <si>
+    <t>TODO: Add rotation</t>
   </si>
 </sst>
 </file>
@@ -631,8 +634,78 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="669">
+  <cellStyleXfs count="739">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1343,7 +1416,7 @@
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="669">
+  <cellStyles count="739">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1678,6 +1751,41 @@
     <cellStyle name="Followed Hyperlink" xfId="664" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="668" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="670" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="672" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="694" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="696" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="700" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="702" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="708" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="710" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="718" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="728" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="730" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="732" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="734" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="736" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="738" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2012,6 +2120,41 @@
     <cellStyle name="Hyperlink" xfId="663" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="665" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="667" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="669" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="671" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="675" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="707" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="709" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="711" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="717" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="725" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="727" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="729" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="731" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="733" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="735" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="737" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -4828,7 +4971,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4850,7 +4993,7 @@
         <v>126</v>
       </c>
       <c r="G1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H1" t="s">
         <v>42</v>
@@ -4862,7 +5005,7 @@
         <v>42</v>
       </c>
       <c r="K1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -4966,14 +5109,14 @@
         <v>120</v>
       </c>
       <c r="C6">
-        <v>-123.8</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
         <v>157</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>-2.1607176139689801</v>
+        <v>0</v>
       </c>
       <c r="F6" t="s">
         <v>157</v>
@@ -4990,14 +5133,14 @@
         <v>121</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>123.8</v>
       </c>
       <c r="D7" t="s">
         <v>157</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.1607176139689801</v>
       </c>
       <c r="F7" t="s">
         <v>157</v>
@@ -5014,14 +5157,14 @@
         <v>120</v>
       </c>
       <c r="C8">
-        <v>-123.8</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>157</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>-2.1607176139689801</v>
+        <v>0</v>
       </c>
       <c r="F8" t="s">
         <v>157</v>
@@ -5035,14 +5178,14 @@
         <v>121</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>123.8</v>
       </c>
       <c r="D9" t="s">
         <v>157</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.1607176139689801</v>
       </c>
       <c r="F9" t="s">
         <v>157</v>
@@ -5059,14 +5202,14 @@
         <v>120</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>-117.1</v>
       </c>
       <c r="D10">
         <v>-27.7</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2.0437805540853597</v>
       </c>
       <c r="F10">
         <f>RADIANS(D10)</f>
@@ -5084,17 +5227,17 @@
         <v>121</v>
       </c>
       <c r="C11">
-        <v>117.1</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>58</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>2.0437805540853597</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <f t="shared" ref="F11:F19" si="1">RADIANS(D11)</f>
+        <f t="shared" ref="F11:F23" si="1">RADIANS(D11)</f>
         <v>1.0122909661567112</v>
       </c>
       <c r="H11" t="s">
@@ -5109,14 +5252,14 @@
         <v>120</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>-117.1</v>
       </c>
       <c r="D12">
         <v>-27.7</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2.0437805540853597</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
@@ -5125,20 +5268,23 @@
       <c r="H12" t="s">
         <v>135</v>
       </c>
+      <c r="I12" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="13" spans="1:11">
       <c r="B13" t="s">
         <v>121</v>
       </c>
       <c r="C13">
-        <v>117.1</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <v>58</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>2.0437805540853597</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
@@ -5300,24 +5446,24 @@
         <v>120</v>
       </c>
       <c r="C20">
-        <v>-63</v>
+        <v>-193.2</v>
       </c>
       <c r="D20">
-        <v>-50.8</v>
+        <v>-132.1</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>-1.0995574287564276</v>
+        <v>-3.3719761148530445</v>
       </c>
       <c r="F20">
-        <f>RADIANS(D21)</f>
-        <v>2.3055799418845093</v>
+        <f t="shared" si="1"/>
+        <v>-2.3055799418845093</v>
       </c>
       <c r="H20" t="s">
         <v>143</v>
       </c>
       <c r="I20" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -5325,18 +5471,18 @@
         <v>121</v>
       </c>
       <c r="C21">
-        <v>193.2</v>
+        <v>63</v>
       </c>
       <c r="D21">
-        <v>132.1</v>
+        <v>50.8</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>3.3719761148530445</v>
+        <v>1.0995574287564276</v>
       </c>
       <c r="F21">
-        <f>RADIANS(D20)</f>
-        <v>-0.88662726001311931</v>
+        <f t="shared" si="1"/>
+        <v>0.88662726001311931</v>
       </c>
       <c r="H21" t="s">
         <v>144</v>
@@ -5350,18 +5496,18 @@
         <v>120</v>
       </c>
       <c r="C22">
-        <v>-63</v>
+        <v>-193.2</v>
       </c>
       <c r="D22">
-        <v>-50.8</v>
+        <v>-132.1</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>-1.0995574287564276</v>
+        <v>-3.3719761148530445</v>
       </c>
       <c r="F22">
-        <f>RADIANS(D22)</f>
-        <v>-0.88662726001311931</v>
+        <f t="shared" si="1"/>
+        <v>-2.3055799418845093</v>
       </c>
       <c r="H22" t="s">
         <v>145</v>
@@ -5372,18 +5518,18 @@
         <v>121</v>
       </c>
       <c r="C23">
-        <v>193.2</v>
+        <v>63</v>
       </c>
       <c r="D23">
-        <v>132.1</v>
+        <v>50.8</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>3.3719761148530445</v>
+        <v>1.0995574287564276</v>
       </c>
       <c r="F23">
-        <f>RADIANS(D23)</f>
-        <v>2.3055799418845093</v>
+        <f t="shared" si="1"/>
+        <v>0.88662726001311931</v>
       </c>
       <c r="H23" t="s">
         <v>146</v>

</xml_diff>

<commit_message>
Reduce friction so model is more solvable with PR2 constraint. Fix shoulder joint limits
</commit_message>
<xml_diff>
--- a/human_measurements.xlsx
+++ b/human_measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="2600" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="10680" yWindow="1300" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Weight" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="165">
   <si>
     <t>Pounds to Kilograms</t>
   </si>
@@ -519,7 +519,7 @@
     <t>Hip cannot go below 0</t>
   </si>
   <si>
-    <t>TODO: Add rotation</t>
+    <t>Roll (Degree)</t>
   </si>
 </sst>
 </file>
@@ -634,8 +634,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="739">
+  <cellStyleXfs count="759">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1416,7 +1436,7 @@
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="739">
+  <cellStyles count="759">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1786,6 +1806,16 @@
     <cellStyle name="Followed Hyperlink" xfId="734" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="736" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="738" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="740" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="742" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="744" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="746" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="748" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="750" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="752" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="754" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="756" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="758" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2155,6 +2185,16 @@
     <cellStyle name="Hyperlink" xfId="733" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="735" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="737" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="739" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="741" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="743" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="745" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="747" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="749" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="751" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="753" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="755" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="757" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -4968,15 +5008,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -4987,28 +5027,31 @@
         <v>124</v>
       </c>
       <c r="E1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" t="s">
         <v>125</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>126</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>162</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>155</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -5021,21 +5064,27 @@
       <c r="D2" t="s">
         <v>157</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2">
         <f>RADIANS(C2)</f>
         <v>-0.68067840827778847</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>157</v>
       </c>
       <c r="H2" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2" t="s">
         <v>122</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="B3" t="s">
         <v>121</v>
       </c>
@@ -5045,18 +5094,24 @@
       <c r="D3" t="s">
         <v>157</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E31" si="0">RADIANS(C3)</f>
+      <c r="E3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F31" si="0">RADIANS(C3)</f>
         <v>0.7260569688296411</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>157</v>
       </c>
       <c r="H3" t="s">
+        <v>157</v>
+      </c>
+      <c r="I3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -5069,18 +5124,24 @@
       <c r="D4" t="s">
         <v>157</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4">
         <f t="shared" si="0"/>
         <v>-0.68067840827778847</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>157</v>
       </c>
       <c r="H4" t="s">
+        <v>157</v>
+      </c>
+      <c r="I4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="B5" t="s">
         <v>121</v>
       </c>
@@ -5090,18 +5151,24 @@
       <c r="D5" t="s">
         <v>157</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="0"/>
         <v>0.7260569688296411</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>157</v>
       </c>
       <c r="H5" t="s">
+        <v>157</v>
+      </c>
+      <c r="I5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>94</v>
       </c>
@@ -5114,21 +5181,27 @@
       <c r="D6" t="s">
         <v>157</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
         <v>157</v>
       </c>
       <c r="H6" t="s">
+        <v>157</v>
+      </c>
+      <c r="I6" t="s">
         <v>129</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="B7" t="s">
         <v>121</v>
       </c>
@@ -5138,18 +5211,24 @@
       <c r="D7" t="s">
         <v>157</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="0"/>
         <v>2.1607176139689801</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>157</v>
       </c>
       <c r="H7" t="s">
+        <v>157</v>
+      </c>
+      <c r="I7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>96</v>
       </c>
@@ -5162,18 +5241,24 @@
       <c r="D8" t="s">
         <v>157</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
         <v>157</v>
       </c>
       <c r="H8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I8" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="B9" t="s">
         <v>121</v>
       </c>
@@ -5183,18 +5268,24 @@
       <c r="D9" t="s">
         <v>157</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="s">
+        <v>157</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="0"/>
         <v>2.1607176139689801</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>157</v>
       </c>
       <c r="H9" t="s">
+        <v>157</v>
+      </c>
+      <c r="I9" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -5208,21 +5299,28 @@
         <v>-27.7</v>
       </c>
       <c r="E10">
+        <v>-34.700000000000003</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="0"/>
         <v>-2.0437805540853597</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <f>RADIANS(D10)</f>
         <v>-0.48345620280242929</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10">
+        <f>RADIANS(E10)</f>
+        <v>-0.60562925044203242</v>
+      </c>
+      <c r="I10" t="s">
         <v>133</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12">
       <c r="B11" t="s">
         <v>121</v>
       </c>
@@ -5233,18 +5331,25 @@
         <v>58</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="F11">
-        <f t="shared" ref="F11:F23" si="1">RADIANS(D11)</f>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:G23" si="1">RADIANS(D11)</f>
         <v>1.0122909661567112</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11">
+        <f>RADIANS(E11)</f>
+        <v>0.67544242052180559</v>
+      </c>
+      <c r="I11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -5258,21 +5363,28 @@
         <v>-27.7</v>
       </c>
       <c r="E12">
+        <v>-34.700000000000003</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="0"/>
         <v>-2.0437805540853597</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <f t="shared" si="1"/>
         <v>-0.48345620280242929</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12">
+        <f>RADIANS(E12)</f>
+        <v>-0.60562925044203242</v>
+      </c>
+      <c r="I12" t="s">
         <v>135</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12">
       <c r="B13" t="s">
         <v>121</v>
       </c>
@@ -5283,18 +5395,25 @@
         <v>58</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="1"/>
         <v>1.0122909661567112</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13">
+        <f>RADIANS(E13)</f>
+        <v>0.67544242052180559</v>
+      </c>
+      <c r="I13" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>102</v>
       </c>
@@ -5308,18 +5427,24 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H14" t="s">
+        <v>157</v>
+      </c>
+      <c r="I14" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12">
       <c r="B15" t="s">
         <v>121</v>
       </c>
@@ -5330,18 +5455,24 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H15" t="s">
+        <v>157</v>
+      </c>
+      <c r="I15" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>104</v>
       </c>
@@ -5355,18 +5486,24 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H16" t="s">
+        <v>157</v>
+      </c>
+      <c r="I16" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="B17" t="s">
         <v>121</v>
       </c>
@@ -5377,18 +5514,24 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H17" t="s">
+        <v>157</v>
+      </c>
+      <c r="I17" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>106</v>
       </c>
@@ -5402,21 +5545,27 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H18" t="s">
+        <v>157</v>
+      </c>
+      <c r="I18" t="s">
         <v>141</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:10">
       <c r="B19" t="s">
         <v>121</v>
       </c>
@@ -5427,18 +5576,24 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H19" t="s">
+        <v>157</v>
+      </c>
+      <c r="I19" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>109</v>
       </c>
@@ -5452,21 +5607,25 @@
         <v>-132.1</v>
       </c>
       <c r="E20">
+        <v>-95.7</v>
+      </c>
+      <c r="F20">
         <f t="shared" si="0"/>
         <v>-3.3719761148530445</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <f t="shared" si="1"/>
         <v>-2.3055799418845093</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20">
+        <f>RADIANS(E20)</f>
+        <v>-1.6702800941585734</v>
+      </c>
+      <c r="I20" t="s">
         <v>143</v>
       </c>
-      <c r="I20" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+    </row>
+    <row r="21" spans="1:10">
       <c r="B21" t="s">
         <v>121</v>
       </c>
@@ -5477,18 +5636,25 @@
         <v>50.8</v>
       </c>
       <c r="E21">
+        <v>30.7</v>
+      </c>
+      <c r="F21">
         <f t="shared" si="0"/>
         <v>1.0995574287564276</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <f t="shared" si="1"/>
         <v>0.88662726001311931</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21">
+        <f>RADIANS(E21)</f>
+        <v>0.53581608036225914</v>
+      </c>
+      <c r="I21" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>111</v>
       </c>
@@ -5502,18 +5668,25 @@
         <v>-132.1</v>
       </c>
       <c r="E22">
+        <v>-95.7</v>
+      </c>
+      <c r="F22">
         <f t="shared" si="0"/>
         <v>-3.3719761148530445</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <f t="shared" si="1"/>
         <v>-2.3055799418845093</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22">
+        <f>RADIANS(E22)</f>
+        <v>-1.6702800941585734</v>
+      </c>
+      <c r="I22" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:10">
       <c r="B23" t="s">
         <v>121</v>
       </c>
@@ -5524,18 +5697,25 @@
         <v>50.8</v>
       </c>
       <c r="E23">
+        <v>30.7</v>
+      </c>
+      <c r="F23">
         <f t="shared" si="0"/>
         <v>1.0995574287564276</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <f t="shared" si="1"/>
         <v>0.88662726001311931</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23">
+        <f>RADIANS(E23)</f>
+        <v>0.53581608036225914</v>
+      </c>
+      <c r="I23" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>113</v>
       </c>
@@ -5548,18 +5728,24 @@
       <c r="D24" t="s">
         <v>157</v>
       </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="E24" t="s">
+        <v>157</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
         <v>157</v>
       </c>
       <c r="H24" t="s">
+        <v>157</v>
+      </c>
+      <c r="I24" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:10">
       <c r="B25" t="s">
         <v>121</v>
       </c>
@@ -5569,18 +5755,24 @@
       <c r="D25" t="s">
         <v>157</v>
       </c>
-      <c r="E25">
+      <c r="E25" t="s">
+        <v>157</v>
+      </c>
+      <c r="F25">
         <f t="shared" si="0"/>
         <v>2.4609142453120048</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>157</v>
       </c>
       <c r="H25" t="s">
+        <v>157</v>
+      </c>
+      <c r="I25" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>115</v>
       </c>
@@ -5593,18 +5785,24 @@
       <c r="D26" t="s">
         <v>157</v>
       </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="E26" t="s">
+        <v>157</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
         <v>157</v>
       </c>
       <c r="H26" t="s">
+        <v>157</v>
+      </c>
+      <c r="I26" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:10">
       <c r="B27" t="s">
         <v>121</v>
       </c>
@@ -5614,18 +5812,24 @@
       <c r="D27" t="s">
         <v>157</v>
       </c>
-      <c r="E27">
+      <c r="E27" t="s">
+        <v>157</v>
+      </c>
+      <c r="F27">
         <f t="shared" si="0"/>
         <v>2.4609142453120048</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>157</v>
       </c>
       <c r="H27" t="s">
+        <v>157</v>
+      </c>
+      <c r="I27" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>117</v>
       </c>
@@ -5638,19 +5842,25 @@
       <c r="D28">
         <v>-25.1</v>
       </c>
-      <c r="E28">
+      <c r="E28" t="s">
+        <v>157</v>
+      </c>
+      <c r="F28">
         <f t="shared" si="0"/>
         <v>-1.6510814723866356</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <f>RADIANS(D28)</f>
         <v>-0.43807764225057672</v>
       </c>
       <c r="H28" t="s">
+        <v>157</v>
+      </c>
+      <c r="I28" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:10">
       <c r="B29" t="s">
         <v>121</v>
       </c>
@@ -5660,19 +5870,25 @@
       <c r="D29">
         <v>46.3</v>
       </c>
-      <c r="E29">
+      <c r="E29" t="s">
+        <v>157</v>
+      </c>
+      <c r="F29">
         <f t="shared" si="0"/>
         <v>1.7802358370342162</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <f>RADIANS(D29)</f>
         <v>0.80808744367337448</v>
       </c>
       <c r="H29" t="s">
+        <v>157</v>
+      </c>
+      <c r="I29" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>119</v>
       </c>
@@ -5685,19 +5901,25 @@
       <c r="D30">
         <v>-25.1</v>
       </c>
-      <c r="E30">
+      <c r="E30" t="s">
+        <v>157</v>
+      </c>
+      <c r="F30">
         <f t="shared" si="0"/>
         <v>-1.6510814723866356</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <f>RADIANS(D30)</f>
         <v>-0.43807764225057672</v>
       </c>
       <c r="H30" t="s">
+        <v>157</v>
+      </c>
+      <c r="I30" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:10">
       <c r="B31" t="s">
         <v>121</v>
       </c>
@@ -5707,15 +5929,21 @@
       <c r="D31">
         <v>46.3</v>
       </c>
-      <c r="E31">
+      <c r="E31" t="s">
+        <v>157</v>
+      </c>
+      <c r="F31">
         <f t="shared" si="0"/>
         <v>1.7802358370342162</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <f>RADIANS(D31)</f>
         <v>0.80808744367337448</v>
       </c>
       <c r="H31" t="s">
+        <v>157</v>
+      </c>
+      <c r="I31" t="s">
         <v>154</v>
       </c>
     </row>

</xml_diff>